<commit_message>
Fixed process for solutionsmanagement
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdehaas\Documents\GIT\Frameworks\October\Performer_Queue\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ciphixinternal-my.sharepoint.com/personal/rwismans_ciphix_io/Documents/Documents/Framework/Repository/uipath-test-pipeline/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6A7EFE-CA0A-4BAB-86C7-91A45FFF8192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{DE6A7EFE-CA0A-4BAB-86C7-91A45FFF8192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F569AFB2-5FDD-411E-BE3A-748AB8DBDB70}"/>
   <bookViews>
-    <workbookView xWindow="8970" yWindow="3525" windowWidth="22410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="251">
   <si>
     <t>Name</t>
   </si>
@@ -864,9 +864,6 @@
     <t>Used in the Orchestrator HTTP requests to work with queues in right folder. If left empty: 'Default' assigned to Cloud Orch, Current job folder assigned to On Prem Orch</t>
   </si>
   <si>
-    <t>TestQueue</t>
-  </si>
-  <si>
     <t>RuntimeReport</t>
   </si>
   <si>
@@ -880,6 +877,24 @@
   </si>
   <si>
     <t>Process Report</t>
+  </si>
+  <si>
+    <t>TestPipelineQueue</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>TestPipelinesAndSolutionsManagement</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>rwismans@ciphix.io</t>
+  </si>
+  <si>
+    <t>CounterAsset</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1002,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1153,6 +1168,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{64123881-3918-4ADD-B104-AD1D75F1F4BE}" name="Tabel9" displayName="Tabel9" ref="A1:C27" totalsRowShown="0">
   <tableColumns count="3">
@@ -1165,7 +1184,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3EA3E27A-FA07-4F2A-9CC0-F39708511072}" name="Tabel8" displayName="Tabel8" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3EA3E27A-FA07-4F2A-9CC0-F39708511072}" name="Tabel8" displayName="Tabel8" ref="A1:D2" totalsRowShown="0" headerRowDxfId="9">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5CB6E98F-B299-4F3D-9F11-FC970305F421}" name="Name"/>
     <tableColumn id="2" xr3:uid="{7C09D0A0-E499-4E6B-BC65-EA3039459FED}" name="Value"/>
@@ -1211,9 +1230,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1251,7 +1270,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1357,7 +1376,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1499,7 +1518,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1510,7 +1529,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,7 +1578,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
@@ -1570,7 +1589,7 @@
         <v>119</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>121</v>
@@ -1580,7 +1599,9 @@
       <c r="A4" t="s">
         <v>235</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>246</v>
+      </c>
       <c r="C4" s="11" t="s">
         <v>239</v>
       </c>
@@ -1590,7 +1611,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>118</v>
+        <v>247</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>15</v>
@@ -1656,7 +1677,7 @@
         <v>154</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>118</v>
+        <v>248</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>155</v>
@@ -1752,7 +1773,7 @@
         <v>58</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>7</v>
@@ -1801,7 +1822,7 @@
         <v>144</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>118</v>
+        <v>249</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>230</v>
@@ -1812,7 +1833,7 @@
         <v>145</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>118</v>
+        <v>249</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>231</v>
@@ -1848,8 +1869,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B24" r:id="rId1" display="aterhaar@ciphix.io" xr:uid="{C07A5796-9FBE-4132-9130-1576CFAE05D8}"/>
-    <hyperlink ref="B25" r:id="rId2" display="aterhaar@ciphix.io" xr:uid="{8721B81B-0325-4655-A32E-26DBE16FE763}"/>
+    <hyperlink ref="B24" r:id="rId1" xr:uid="{C07A5796-9FBE-4132-9130-1576CFAE05D8}"/>
+    <hyperlink ref="B25" r:id="rId2" xr:uid="{8721B81B-0325-4655-A32E-26DBE16FE763}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1875,7 +1896,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X991"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1918,6 +1941,14 @@
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
+    </row>
+    <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="3" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3658,13 +3689,13 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>242</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>